<commit_message>
stored npy arrays of mocap waypoints
</commit_message>
<xml_diff>
--- a/Data analytics/data descriptions.xlsx
+++ b/Data analytics/data descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spiest\2023Summer\LUCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\projects\ChessRobot\Data analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739119B6-BCB7-437A-B7E4-FFEC8F14B804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2B5888-E043-4413-8C65-7E071D6B0A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{04F88386-A33D-43E8-96F0-AEE909C03856}"/>
+    <workbookView xWindow="2453" yWindow="2453" windowWidth="21600" windowHeight="11295" xr2:uid="{04F88386-A33D-43E8-96F0-AEE909C03856}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>record of data</t>
   </si>
@@ -85,14 +85,37 @@
   </si>
   <si>
     <t>Sagging with further distance. Home was assumed as correct</t>
+  </si>
+  <si>
+    <t>numpy array of waypoints title</t>
+  </si>
+  <si>
+    <t>path_board</t>
+  </si>
+  <si>
+    <t>path_bigXs</t>
+  </si>
+  <si>
+    <t>path_midXs</t>
+  </si>
+  <si>
+    <t>path_smallXs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,9 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -146,14 +172,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>551505</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>151363</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>260909</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2095500</xdr:rowOff>
     </xdr:to>
@@ -178,8 +204,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9471660" y="4785360"/>
-          <a:ext cx="2757403" cy="2004060"/>
+          <a:off x="10814693" y="5139690"/>
+          <a:ext cx="2876466" cy="2004060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -190,14 +216,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>274321</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>383866</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>122684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>452446</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>38653</xdr:rowOff>
     </xdr:to>
@@ -222,8 +248,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9304021" y="6980684"/>
-          <a:ext cx="2506980" cy="2080049"/>
+          <a:off x="10647054" y="7333109"/>
+          <a:ext cx="2602230" cy="2078144"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -234,14 +260,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>487681</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>149551</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>240990</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>2144577</xdr:rowOff>
     </xdr:to>
@@ -266,8 +292,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9517381" y="9037320"/>
-          <a:ext cx="2529839" cy="2129337"/>
+          <a:off x="10412739" y="9387840"/>
+          <a:ext cx="2625089" cy="2129337"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -576,48 +602,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A3AC8F-E044-4904-8A43-B90970DE6318}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
     <col min="2" max="2" width="26.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="29.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" style="1" customWidth="1"/>
+    <col min="5" max="10" width="8.86328125" style="1"/>
+    <col min="11" max="11" width="12.19921875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -645,8 +676,11 @@
       <c r="J2" s="1">
         <v>260</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -674,8 +708,11 @@
       <c r="J3" s="1">
         <v>260</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -703,8 +740,11 @@
       <c r="J4" s="1">
         <v>340</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -732,8 +772,11 @@
       <c r="J5" s="1">
         <v>520</v>
       </c>
+      <c r="K5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -761,24 +804,28 @@
       <c r="J6" s="1">
         <v>520</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="170.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="67.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="1:11" ht="170.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:11" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" ht="67.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>